<commit_message>
added title to charts
</commit_message>
<xml_diff>
--- a/assignment4/HeatForOMP/Thread_Affinity/KMP_results.xlsx
+++ b/assignment4/HeatForOMP/Thread_Affinity/KMP_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/734b88e09210c75b/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hemra\Downloads\Programming_of_supercomputer\pos_21_group12\assignment4\HeatForOMP\Thread_Affinity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="401" documentId="8_{02AF128C-B6E5-4477-9BF9-7D181EA5D3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{244CB470-23DE-43B7-8E5B-9602BADFD14F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AED999-4831-4A20-A48A-80BEF8B0ADDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{896928AA-22C5-4A85-AB0D-4E782E40DBA7}"/>
   </bookViews>
@@ -91,14 +91,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -130,7 +130,67 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speedup -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Thread Affinity</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -347,7 +407,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -585,7 +644,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -673,7 +732,62 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Performance - Thread Affinity</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1127,7 +1241,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2705,18 +2819,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2765,8 +2879,8 @@
         <f>$E$3/E3</f>
         <v>1</v>
       </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2792,8 +2906,8 @@
         <f t="shared" ref="G4:G11" si="1">$E$3/E4</f>
         <v>1.5973997050427906</v>
       </c>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -2819,8 +2933,8 @@
         <f t="shared" si="1"/>
         <v>3.0301757893001406</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -2846,8 +2960,8 @@
         <f t="shared" si="1"/>
         <v>4.9717659788498443</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -2873,8 +2987,8 @@
         <f t="shared" si="1"/>
         <v>6.4451774452486754</v>
       </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2900,8 +3014,8 @@
         <f t="shared" si="1"/>
         <v>6.8137399716164158</v>
       </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2927,8 +3041,8 @@
         <f t="shared" si="1"/>
         <v>7.1147146347954422</v>
       </c>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2954,8 +3068,8 @@
         <f t="shared" si="1"/>
         <v>7.1923227431702008</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2981,28 +3095,28 @@
         <f t="shared" si="1"/>
         <v>6.7223870020173626</v>
       </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="K15" s="1" t="s">
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="K15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="P15" s="1" t="s">
+      <c r="L15" s="5"/>
+      <c r="P15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Q15" s="1"/>
+      <c r="Q15" s="5"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -3069,18 +3183,18 @@
         <f>$E$17/E17</f>
         <v>1</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="4">
         <v>1</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="3">
         <f>$B$17/B17</f>
         <v>1</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="3">
         <f>$E$17/E17</f>
         <v>1</v>
       </c>
-      <c r="O17" s="5">
+      <c r="O17" s="4">
         <v>1</v>
       </c>
       <c r="P17">
@@ -3114,18 +3228,18 @@
         <f t="shared" ref="G18:G25" si="3">$E$17/E18</f>
         <v>1.5972357579516256</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="4">
         <v>2</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="3">
         <f t="shared" ref="K18:K25" si="4">$B$17/B18</f>
         <v>1.0965501163327445</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="3">
         <f t="shared" ref="L18:L25" si="5">$E$17/E18</f>
         <v>1.5972357579516256</v>
       </c>
-      <c r="O18" s="5">
+      <c r="O18" s="4">
         <v>2</v>
       </c>
       <c r="P18">
@@ -3159,18 +3273,18 @@
         <f t="shared" si="3"/>
         <v>2.9912760325521948</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19" s="4">
         <v>4</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="3">
         <f t="shared" si="4"/>
         <v>2.1008182516570493</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19" s="3">
         <f t="shared" si="5"/>
         <v>2.9912760325521948</v>
       </c>
-      <c r="O19" s="5">
+      <c r="O19" s="4">
         <v>4</v>
       </c>
       <c r="P19">
@@ -3204,18 +3318,18 @@
         <f t="shared" si="3"/>
         <v>4.8866921633652245</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20" s="4">
         <v>8</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="3">
         <f t="shared" si="4"/>
         <v>3.673075361250461</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="3">
         <f t="shared" si="5"/>
         <v>4.8866921633652245</v>
       </c>
-      <c r="O20" s="5">
+      <c r="O20" s="4">
         <v>8</v>
       </c>
       <c r="P20">
@@ -3249,18 +3363,18 @@
         <f t="shared" si="3"/>
         <v>6.1873153257506281</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21" s="4">
         <v>12</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="3">
         <f t="shared" si="4"/>
         <v>4.4313714406307003</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="3">
         <f t="shared" si="5"/>
         <v>6.1873153257506281</v>
       </c>
-      <c r="O21" s="5">
+      <c r="O21" s="4">
         <v>12</v>
       </c>
       <c r="P21">
@@ -3294,18 +3408,18 @@
         <f t="shared" si="3"/>
         <v>6.6041543841975416</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J22" s="4">
         <v>16</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="3">
         <f t="shared" si="4"/>
         <v>4.952767446856007</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="3">
         <f t="shared" si="5"/>
         <v>6.6041543841975416</v>
       </c>
-      <c r="O22" s="5">
+      <c r="O22" s="4">
         <v>16</v>
       </c>
       <c r="P22">
@@ -3339,18 +3453,18 @@
         <f t="shared" si="3"/>
         <v>6.6732910345465797</v>
       </c>
-      <c r="J23" s="5">
+      <c r="J23" s="4">
         <v>24</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="3">
         <f t="shared" si="4"/>
         <v>5.5474930178140101</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="3">
         <f t="shared" si="5"/>
         <v>6.6732910345465797</v>
       </c>
-      <c r="O23" s="5">
+      <c r="O23" s="4">
         <v>24</v>
       </c>
       <c r="P23">
@@ -3384,18 +3498,18 @@
         <f t="shared" si="3"/>
         <v>7.1949663571566651</v>
       </c>
-      <c r="J24" s="5">
+      <c r="J24" s="4">
         <v>32</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="3">
         <f t="shared" si="4"/>
         <v>6.0591387599255935</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="3">
         <f t="shared" si="5"/>
         <v>7.1949663571566651</v>
       </c>
-      <c r="O24" s="5">
+      <c r="O24" s="4">
         <v>32</v>
       </c>
       <c r="P24">
@@ -3429,18 +3543,18 @@
         <f t="shared" si="3"/>
         <v>6.577386585185101</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J25" s="4">
         <v>48</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K25" s="3">
         <f t="shared" si="4"/>
         <v>5.6003343366608247</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25" s="3">
         <f t="shared" si="5"/>
         <v>6.577386585185101</v>
       </c>
-      <c r="O25" s="5">
+      <c r="O25" s="4">
         <v>48</v>
       </c>
       <c r="P25">
@@ -3451,16 +3565,16 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1" t="s">
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -3675,17 +3789,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3936,17 +4050,17 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1" t="s">
+      <c r="A15" s="2"/>
+      <c r="B15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -4128,7 +4242,7 @@
       <c r="B23">
         <v>0.21573400000000001</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>27418</v>
       </c>
       <c r="D23">
@@ -4197,16 +4311,16 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1" t="s">
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">

</xml_diff>